<commit_message>
project population to 1470
</commit_message>
<xml_diff>
--- a/projection/csv/population_projection.xlsx
+++ b/projection/csv/population_projection.xlsx
@@ -142,23 +142,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,10 +239,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -666,6 +666,166 @@
         <v>93412</v>
       </c>
     </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="n">
+        <v>1451</v>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>93401</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="n">
+        <v>1452</v>
+      </c>
+      <c r="B54" s="4" t="n">
+        <v>93390</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="n">
+        <v>1453</v>
+      </c>
+      <c r="B55" s="4" t="n">
+        <v>93379</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="n">
+        <v>1454</v>
+      </c>
+      <c r="B56" s="4" t="n">
+        <v>93368</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="n">
+        <v>1455</v>
+      </c>
+      <c r="B57" s="4" t="n">
+        <v>93357</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="n">
+        <v>1456</v>
+      </c>
+      <c r="B58" s="4" t="n">
+        <v>93346</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="n">
+        <v>1457</v>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>93335</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="n">
+        <v>1458</v>
+      </c>
+      <c r="B60" s="4" t="n">
+        <v>93324</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="n">
+        <v>1459</v>
+      </c>
+      <c r="B61" s="4" t="n">
+        <v>93313</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="n">
+        <v>1460</v>
+      </c>
+      <c r="B62" s="4" t="n">
+        <v>93302</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="n">
+        <v>1461</v>
+      </c>
+      <c r="B63" s="4" t="n">
+        <v>93291</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="n">
+        <v>1462</v>
+      </c>
+      <c r="B64" s="4" t="n">
+        <v>93280</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="n">
+        <v>1463</v>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>93269</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="n">
+        <v>1464</v>
+      </c>
+      <c r="B66" s="4" t="n">
+        <v>93258</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="n">
+        <v>1465</v>
+      </c>
+      <c r="B67" s="4" t="n">
+        <v>93247</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="n">
+        <v>1466</v>
+      </c>
+      <c r="B68" s="4" t="n">
+        <v>93236</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="n">
+        <v>1467</v>
+      </c>
+      <c r="B69" s="4" t="n">
+        <v>93225</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="n">
+        <v>1468</v>
+      </c>
+      <c r="B70" s="4" t="n">
+        <v>93214</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="n">
+        <v>1469</v>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>93203</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="n">
+        <v>1470</v>
+      </c>
+      <c r="B72" s="4" t="n">
+        <v>93192</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>